<commit_message>
Personal Health Records - regenerate outputs Event Summary - regenerate outputs Shared Health Summary - regenerate outputs
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -557,7 +557,7 @@
   <si>
     <t>One would expect this element to be a cardinality  of 1..1.  The only circumstance in which the subject can be missing is when the observation is made by a device that does not know the patient. In this case, the observation SHALL be matched to a patient through some context/channel matching technique, and at this point, the observation should be updated. -If the target of the observation is different than the subject, the general extension [observation-focal-subject](http://hl7.org/fhir/STU3/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
+If the target of the observation is different than the subject, the general extension [observation-focal-subject](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-observation-focal-subject.html).  may be used.  However, the distinction between the patient's own value for an observation versus that of the fetus, or the donor or blood product unit, etc., are often specified in the observation code.</t>
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
@@ -713,7 +713,7 @@
     <t>Normally, an observation will have either a single value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and related observations (for an Apgar score, the observations from which the measure is derived). If a value is present, the datatype for this element should be determined by Observation.code. This element has a variable name depending on the type as follows: valueQuantity, valueCodeableConcept, valueString, valueBoolean, valueRange, valueRatio, valueSampledData, valueAttachment, valueTime, valueDateTime, or valuePeriod. (The name format is "'value' + the type name" with a capital on the first letter of the type).  -If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+If the data element is usually coded or if the type associated with the Observation.value defines a coded value, use CodeableConcept instead of string datatype even if the value is uncoded text.  A value set is bound to the ValueCodeableConcept element.    For further discussion and examples see the  [notes section](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
@@ -840,7 +840,7 @@
     <t>Indicates the site on the subject's body where the observation was made (i.e. the target site).</t>
   </si>
   <si>
-    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](http://hl7.org/fhir/STU3/extension-body-site-instance.html).</t>
+    <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-body-site-instance.html).</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1139,7 +1139,7 @@
     <t>A  reference to another resource (usually another Observation) whose relationship is defined by the relationship type code.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](http://hl7.org/fhir/STU3/observation.html#4.20.4).</t>
+    <t>For a discussion on the ways Observations can assembled in groups together see [Notes below](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#4.20.4).</t>
   </si>
   <si>
     <t>Normally, an observation will have either a value or a set of related observations. A few observations (e.g. Apgar score) may have both a value and a set of related observations or sometimes a QuestionnaireResponse from which the measure is derived.</t>
@@ -1198,7 +1198,7 @@
     <t>Resource that is related to this one</t>
   </si>
   <si>
-    <t>A reference to the observation or [QuestionnaireResponse](http://hl7.org/fhir/STU3/questionnaireresponse.html#) resource that is related to this observation.</t>
+    <t>A reference to the observation or [QuestionnaireResponse](https://build.fhir.org/ig/hl7au/au-fhir-base/questionnaireresponse.html#) resource that is related to this observation.</t>
   </si>
   <si>
     <t>.targetObservation</t>
@@ -1213,7 +1213,7 @@
     <t>Some observations have multiple component observations.  These component observations are expressed as separate code value pairs that share the same attributes.  Examples include systolic and diastolic component observations for blood pressure measurement and multiple component observations for genetics observations.</t>
   </si>
   <si>
-    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](http://hl7.org/fhir/STU3/observation.html#notes) below.</t>
+    <t>For a discussion on the ways Observations can be assembled in groups together see [Notes](https://build.fhir.org/ig/hl7au/au-fhir-base/observation.html#notes) below.</t>
   </si>
   <si>
     <t>Component observations share the same attributes in the Observation resource as the primary observation and are always treated a part of a single observation (they are not separable).   However, the reference range for the primary observation value is not inherited by the component values and is required when appropriate for each component observation.</t>

</xml_diff>

<commit_message>
Regenerated IG outputs following improvements to patient profiles
Added a number of invariants to 3 patient profiles and some narrative updates. Regenerated the following IG's:
- Advanced Care Records
- Event Summary
- Personal Health Records
- Shared Health Summary
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$54</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
   <si>
     <t>Path</t>
   </si>
@@ -702,13 +702,10 @@
     <t>who.actor</t>
   </si>
   <si>
-    <t>Observation.valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Coded value of the observation</t>
+    <t>Observation.value[x]</t>
+  </si>
+  <si>
+    <t>Actual result</t>
   </si>
   <si>
     <t>The information determined as a result of making the observation, if the information has a simple value.</t>
@@ -723,10 +720,11 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
-  </si>
-  <si>
-    <t>Observation.value[x]</t>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -746,6 +744,15 @@
   </si>
   <si>
     <t>363714003 |Interprets|</t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Coded value of the observation</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1434,7 +1441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO53"/>
+  <dimension ref="A1:AO54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3842,25 +3849,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="B21" t="s" s="2">
-        <v>218</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3872,16 +3877,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3906,29 +3911,29 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD21" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="Z21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AE21" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3937,68 +3942,70 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AK21" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="AN21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO21" t="s" s="2">
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>230</v>
       </c>
-    </row>
-    <row r="22" hidden="true">
-      <c r="A22" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4023,13 +4030,11 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="X22" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4047,7 +4052,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4056,44 +4061,44 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AL22" t="s" s="2">
-        <v>99</v>
+        <v>227</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>45</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4108,14 +4113,16 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="N23" t="s" s="2">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4143,10 +4150,10 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4164,7 +4171,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4173,37 +4180,37 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>248</v>
+        <v>99</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4222,17 +4229,17 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>252</v>
+        <v>142</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4257,13 +4264,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4281,7 +4288,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4296,27 +4303,27 @@
         <v>45</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>45</v>
+        <v>249</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>45</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4339,18 +4346,18 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>142</v>
+        <v>254</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="N25" s="2"/>
+        <v>256</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" t="s" s="2">
+        <v>257</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4374,13 +4381,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>264</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4398,7 +4405,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4413,27 +4420,27 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>268</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4459,17 +4466,15 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>273</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4496,10 +4501,10 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4517,7 +4522,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4535,24 +4540,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4575,18 +4580,20 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>279</v>
+        <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>275</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4610,13 +4617,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>45</v>
+        <v>276</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>45</v>
+        <v>277</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4634,7 +4641,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4652,24 +4659,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>283</v>
+        <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>286</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4692,16 +4699,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4751,7 +4758,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4769,24 +4776,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4797,7 +4804,7 @@
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4809,20 +4816,18 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4870,42 +4875,42 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="AF29" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>304</v>
-      </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>45</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4916,7 +4921,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -4928,16 +4933,20 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -4985,19 +4994,19 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>45</v>
+        <v>304</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>45</v>
@@ -5006,10 +5015,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5020,18 +5029,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5043,17 +5052,15 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5102,13 +5109,13 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
@@ -5126,7 +5133,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5137,11 +5144,11 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -5154,19 +5161,19 @@
         <v>45</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5219,7 +5226,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5243,7 +5250,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5254,38 +5261,40 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>318</v>
+        <v>102</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>319</v>
+        <v>108</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5334,16 +5343,16 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>45</v>
@@ -5355,10 +5364,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>322</v>
+        <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>323</v>
+        <v>99</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5369,7 +5378,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5392,13 +5401,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5449,7 +5458,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5458,7 +5467,7 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>45</v>
@@ -5470,10 +5479,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5484,7 +5493,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5507,20 +5516,16 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>142</v>
+        <v>320</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>332</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5544,13 +5549,13 @@
         <v>45</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>45</v>
@@ -5568,7 +5573,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5577,7 +5582,7 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>45</v>
@@ -5586,13 +5591,13 @@
         <v>45</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>335</v>
+        <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>249</v>
+        <v>329</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5603,7 +5608,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5614,7 +5619,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
@@ -5629,16 +5634,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5663,13 +5668,13 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
@@ -5687,31 +5692,31 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AF36" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>335</v>
-      </c>
       <c r="AL36" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5722,7 +5727,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5733,7 +5738,7 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5745,17 +5750,19 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>345</v>
+        <v>142</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>342</v>
+      </c>
       <c r="N37" t="s" s="2">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5780,13 +5787,13 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>45</v>
+        <v>344</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>45</v>
+        <v>345</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5804,13 +5811,13 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>45</v>
@@ -5822,13 +5829,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>45</v>
+        <v>337</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>349</v>
+        <v>251</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5839,7 +5846,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5862,16 +5869,18 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>252</v>
+        <v>347</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="N38" t="s" s="2">
+        <v>350</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5919,7 +5928,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5940,10 +5949,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>322</v>
+        <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5954,7 +5963,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5965,7 +5974,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -5974,23 +5983,19 @@
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>358</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6038,19 +6043,19 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>45</v>
@@ -6059,10 +6064,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>360</v>
+        <v>324</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6073,7 +6078,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6084,7 +6089,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6093,19 +6098,23 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>306</v>
+        <v>357</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6153,19 +6162,19 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6174,10 +6183,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>309</v>
+        <v>363</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6188,18 +6197,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6211,17 +6220,15 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6270,13 +6277,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6294,7 +6301,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6305,11 +6312,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6322,19 +6329,19 @@
         <v>45</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6387,7 +6394,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6411,7 +6418,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6422,43 +6429,41 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>366</v>
+        <v>108</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>367</v>
+        <v>317</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>369</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6482,13 +6487,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>371</v>
+        <v>45</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6506,13 +6511,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>365</v>
+        <v>318</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6527,10 +6532,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>372</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6541,7 +6546,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6549,7 +6554,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>56</v>
@@ -6564,16 +6569,20 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>374</v>
+        <v>75</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>371</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6597,13 +6606,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>45</v>
+        <v>372</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6621,10 +6630,10 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>56</v>
@@ -6642,10 +6651,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6656,7 +6665,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6664,10 +6673,10 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6676,23 +6685,19 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>297</v>
+        <v>376</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>382</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6740,19 +6745,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6761,10 +6766,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>383</v>
+        <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6775,7 +6780,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6786,7 +6791,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6795,19 +6800,23 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>306</v>
+        <v>381</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>384</v>
+      </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6855,19 +6864,19 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>308</v>
+        <v>380</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6876,10 +6885,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>45</v>
+        <v>385</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>309</v>
+        <v>386</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6890,18 +6899,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
@@ -6913,17 +6922,15 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6972,13 +6979,13 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
@@ -6996,7 +7003,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7007,11 +7014,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7024,19 +7031,19 @@
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7089,7 +7096,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7113,7 +7120,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7124,41 +7131,41 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>57</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>389</v>
+        <v>108</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" t="s" s="2">
-        <v>156</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7182,13 +7189,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7206,13 +7213,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>388</v>
+        <v>318</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7224,16 +7231,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>391</v>
+        <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>163</v>
+        <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>164</v>
+        <v>99</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7241,7 +7248,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7249,7 +7256,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>56</v>
@@ -7264,19 +7271,17 @@
         <v>57</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>393</v>
+        <v>142</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>395</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7301,13 +7306,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7325,10 +7330,10 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>56</v>
@@ -7343,24 +7348,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>228</v>
+        <v>163</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>229</v>
+        <v>164</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>230</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7380,22 +7385,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>142</v>
+        <v>395</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7420,13 +7425,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>236</v>
+        <v>45</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7444,7 +7449,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7453,7 +7458,7 @@
         <v>56</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>238</v>
+        <v>45</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>45</v>
@@ -7462,28 +7467,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>45</v>
+        <v>398</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>99</v>
+        <v>227</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>45</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7505,16 +7510,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>242</v>
+        <v>400</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7542,10 +7547,10 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7563,7 +7568,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7572,7 +7577,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7581,19 +7586,19 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>248</v>
+        <v>99</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" hidden="true">
@@ -7602,14 +7607,14 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7621,19 +7626,19 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L53" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>300</v>
-      </c>
       <c r="N53" t="s" s="2">
-        <v>301</v>
+        <v>246</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7658,13 +7663,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7688,35 +7693,154 @@
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F54" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="AH53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL53" t="s" s="2">
+      <c r="G54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N54" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="AM53" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO53" t="s" s="2">
+      <c r="O54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO54" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO53">
+  <autoFilter ref="A1:AO54">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7726,7 +7850,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI52">
+  <conditionalFormatting sqref="A2:AI53">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated outputs for following implementation guides which contain updates disclaimers.md page
Advanace Cae Records
Event Summary
Personal Health Records
Presciption Dispense Lists
Shared Health Summary

CIFMM-2613
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="404">
   <si>
     <t>Path</t>
   </si>
@@ -702,10 +702,13 @@
     <t>who.actor</t>
   </si>
   <si>
-    <t>Observation.value[x]</t>
-  </si>
-  <si>
-    <t>Actual result</t>
+    <t>Observation.valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Coded value of the observation</t>
   </si>
   <si>
     <t>The information determined as a result of making the observation, if the information has a simple value.</t>
@@ -720,11 +723,10 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
+  </si>
+  <si>
+    <t>Observation.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -744,15 +746,6 @@
   </si>
   <si>
     <t>363714003 |Interprets|</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Coded value of the observation</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1441,7 +1434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO54"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3849,23 +3842,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" t="s" s="2">
+        <v>218</v>
+      </c>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3877,16 +3872,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3911,29 +3906,29 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X21" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="X21" s="2"/>
       <c r="Y21" t="s" s="2">
-        <v>45</v>
+        <v>223</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AB21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>223</v>
+        <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3942,70 +3937,68 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4030,11 +4023,13 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X22" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="Y22" t="s" s="2">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4052,7 +4047,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4061,44 +4056,44 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>227</v>
+        <v>99</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>229</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4113,16 +4108,14 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4150,10 +4143,10 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4171,7 +4164,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4180,37 +4173,37 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>99</v>
+        <v>248</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>243</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4229,17 +4222,17 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4264,13 +4257,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4288,7 +4281,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4303,27 +4296,27 @@
         <v>45</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>252</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4346,18 +4339,18 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>254</v>
+        <v>142</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" t="s" s="2">
-        <v>257</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4381,13 +4374,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4405,7 +4398,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4420,27 +4413,27 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>45</v>
+        <v>265</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4466,15 +4459,17 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N26" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4501,10 +4496,10 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4522,7 +4517,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4540,24 +4535,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4580,20 +4575,18 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>275</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4617,13 +4610,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>277</v>
+        <v>45</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4641,7 +4634,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4659,24 +4652,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>45</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4699,16 +4692,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4758,7 +4751,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4776,24 +4769,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4804,7 +4797,7 @@
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4816,18 +4809,20 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4875,42 +4870,42 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>297</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4921,7 +4916,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -4933,20 +4928,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>303</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -4994,19 +4985,19 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>304</v>
+        <v>45</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>45</v>
@@ -5015,10 +5006,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>305</v>
+        <v>45</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5029,18 +5020,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5052,15 +5043,17 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5109,13 +5102,13 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
@@ -5133,7 +5126,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5144,11 +5137,11 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -5161,19 +5154,19 @@
         <v>45</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J32" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5226,7 +5219,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5250,7 +5243,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5261,40 +5254,38 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>102</v>
+        <v>318</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>108</v>
+        <v>319</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5343,16 +5334,16 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>45</v>
@@ -5364,10 +5355,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>45</v>
+        <v>322</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>99</v>
+        <v>323</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5378,7 +5369,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5401,13 +5392,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5458,7 +5449,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5467,7 +5458,7 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>45</v>
@@ -5479,10 +5470,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5493,7 +5484,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5516,16 +5507,20 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>320</v>
+        <v>142</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>332</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5549,13 +5544,13 @@
         <v>45</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>45</v>
+        <v>334</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>45</v>
@@ -5573,7 +5568,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5582,7 +5577,7 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>323</v>
+        <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>45</v>
@@ -5591,13 +5586,13 @@
         <v>45</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>45</v>
+        <v>335</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>329</v>
+        <v>249</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5608,7 +5603,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5619,7 +5614,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
@@ -5634,16 +5629,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5668,55 +5663,55 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE36" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="Y36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="Z36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="AF36" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="AL36" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="AM36" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5727,7 +5722,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5738,7 +5733,7 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5750,19 +5745,17 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>142</v>
+        <v>345</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>342</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5787,37 +5780,37 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE37" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>339</v>
-      </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>45</v>
@@ -5829,13 +5822,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>337</v>
+        <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>338</v>
+        <v>45</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>251</v>
+        <v>349</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5846,7 +5839,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5869,18 +5862,16 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>347</v>
+        <v>252</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" t="s" s="2">
-        <v>350</v>
-      </c>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5928,7 +5919,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5949,10 +5940,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>45</v>
+        <v>322</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5963,7 +5954,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5974,7 +5965,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -5983,19 +5974,23 @@
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>358</v>
+      </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6043,19 +6038,19 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>45</v>
@@ -6064,10 +6059,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6078,7 +6073,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6089,7 +6084,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6098,23 +6093,19 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>357</v>
+        <v>306</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6162,19 +6153,19 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6183,10 +6174,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>362</v>
+        <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>363</v>
+        <v>309</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6197,18 +6188,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6220,15 +6211,17 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6277,13 +6270,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6301,7 +6294,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6312,11 +6305,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6329,19 +6322,19 @@
         <v>45</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J42" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6394,7 +6387,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6418,7 +6411,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6429,41 +6422,43 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>108</v>
+        <v>366</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>367</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N43" s="2"/>
+        <v>368</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>369</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6487,13 +6482,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>45</v>
+        <v>370</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>45</v>
+        <v>371</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6511,13 +6506,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>318</v>
+        <v>365</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6532,10 +6527,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>99</v>
+        <v>372</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6546,7 +6541,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6554,7 +6549,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>56</v>
@@ -6569,20 +6564,16 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>75</v>
+        <v>374</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>371</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6606,34 +6597,34 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>372</v>
+        <v>45</v>
       </c>
       <c r="Y44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE44" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="Z44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>367</v>
-      </c>
       <c r="AF44" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>56</v>
@@ -6651,10 +6642,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6665,7 +6656,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6673,10 +6664,10 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6685,19 +6676,23 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>376</v>
+        <v>297</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>380</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>382</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6745,19 +6740,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6766,10 +6761,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>45</v>
+        <v>383</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6780,7 +6775,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6791,7 +6786,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6800,23 +6795,19 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>381</v>
+        <v>306</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>384</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6864,19 +6855,19 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>380</v>
+        <v>308</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6885,10 +6876,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>385</v>
+        <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>386</v>
+        <v>309</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6899,18 +6890,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
@@ -6922,15 +6913,17 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M47" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6979,13 +6972,13 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
@@ -7003,7 +6996,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7014,11 +7007,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7031,19 +7024,19 @@
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J48" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7096,7 +7089,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7120,7 +7113,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7131,41 +7124,41 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>57</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>108</v>
+        <v>389</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N49" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7189,13 +7182,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7213,13 +7206,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7231,16 +7224,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>45</v>
+        <v>391</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7248,7 +7241,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7256,7 +7249,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>56</v>
@@ -7271,17 +7264,19 @@
         <v>57</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>142</v>
+        <v>393</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="M50" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>395</v>
+      </c>
       <c r="N50" t="s" s="2">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7306,13 +7301,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7330,10 +7325,10 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>56</v>
@@ -7348,24 +7343,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7385,22 +7380,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>395</v>
+        <v>142</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7425,13 +7420,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>45</v>
+        <v>236</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>45</v>
+        <v>237</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7449,7 +7444,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7458,7 +7453,7 @@
         <v>56</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>45</v>
@@ -7467,28 +7462,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>398</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>227</v>
+        <v>99</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>229</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7510,16 +7505,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>400</v>
+        <v>242</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7547,10 +7542,10 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7568,7 +7563,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7577,7 +7572,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7586,19 +7581,19 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>99</v>
+        <v>248</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" hidden="true">
@@ -7607,14 +7602,14 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>243</v>
+        <v>45</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7626,19 +7621,19 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>244</v>
+        <v>403</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>403</v>
+        <v>300</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>246</v>
+        <v>301</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7663,13 +7658,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7693,7 +7688,7 @@
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>45</v>
@@ -7705,142 +7700,23 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>251</v>
+        <v>304</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO54" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO54">
+  <autoFilter ref="A1:AO53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7850,7 +7726,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI53">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated outputs for following implementation guides which contain PractitionerRole Invariants added CIFMM-2694
Advanace Cae Records
Event Summary
Shared Health Summary
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$54</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
   <si>
     <t>Path</t>
   </si>
@@ -702,13 +702,10 @@
     <t>who.actor</t>
   </si>
   <si>
-    <t>Observation.valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Coded value of the observation</t>
+    <t>Observation.value[x]</t>
+  </si>
+  <si>
+    <t>Actual result</t>
   </si>
   <si>
     <t>The information determined as a result of making the observation, if the information has a simple value.</t>
@@ -723,10 +720,11 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
-  </si>
-  <si>
-    <t>Observation.value[x]</t>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -746,6 +744,15 @@
   </si>
   <si>
     <t>363714003 |Interprets|</t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Coded value of the observation</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1434,7 +1441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO53"/>
+  <dimension ref="A1:AO54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3842,25 +3849,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="B21" t="s" s="2">
-        <v>218</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3872,16 +3877,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3906,29 +3911,29 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AB21" s="2"/>
+      <c r="AC21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD21" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="Z21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AE21" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3937,68 +3942,70 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AK21" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="AN21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO21" t="s" s="2">
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>230</v>
       </c>
-    </row>
-    <row r="22" hidden="true">
-      <c r="A22" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4023,13 +4030,11 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="X22" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4047,7 +4052,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4056,44 +4061,44 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AL22" t="s" s="2">
-        <v>99</v>
+        <v>227</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>45</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4108,14 +4113,16 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="N23" t="s" s="2">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4143,10 +4150,10 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4164,7 +4171,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4173,37 +4180,37 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>248</v>
+        <v>99</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4222,17 +4229,17 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>252</v>
+        <v>142</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4257,13 +4264,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4281,7 +4288,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4296,27 +4303,27 @@
         <v>45</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>45</v>
+        <v>249</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>45</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4339,18 +4346,18 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>142</v>
+        <v>254</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="N25" s="2"/>
+        <v>256</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" t="s" s="2">
+        <v>257</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4374,13 +4381,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>264</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4398,7 +4405,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4413,27 +4420,27 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>268</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4459,17 +4466,15 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>273</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4496,10 +4501,10 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4517,7 +4522,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4535,24 +4540,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4575,18 +4580,20 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>279</v>
+        <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>275</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4610,13 +4617,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>45</v>
+        <v>276</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>45</v>
+        <v>277</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4634,7 +4641,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4652,24 +4659,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>283</v>
+        <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>286</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4692,16 +4699,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4751,7 +4758,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4769,24 +4776,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4797,7 +4804,7 @@
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4809,20 +4816,18 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4870,42 +4875,42 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="AF29" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>304</v>
-      </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>45</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4916,7 +4921,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -4928,16 +4933,20 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -4985,19 +4994,19 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>45</v>
+        <v>304</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>45</v>
@@ -5006,10 +5015,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5020,18 +5029,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5043,17 +5052,15 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5102,13 +5109,13 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
@@ -5126,7 +5133,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5137,11 +5144,11 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -5154,19 +5161,19 @@
         <v>45</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5219,7 +5226,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5243,7 +5250,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5254,38 +5261,40 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>318</v>
+        <v>102</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>319</v>
+        <v>108</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5334,16 +5343,16 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>45</v>
@@ -5355,10 +5364,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>322</v>
+        <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>323</v>
+        <v>99</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5369,7 +5378,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5392,13 +5401,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5449,7 +5458,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5458,7 +5467,7 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>45</v>
@@ -5470,10 +5479,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5484,7 +5493,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5507,20 +5516,16 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>142</v>
+        <v>320</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>332</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5544,13 +5549,13 @@
         <v>45</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>45</v>
@@ -5568,7 +5573,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5577,7 +5582,7 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>45</v>
@@ -5586,13 +5591,13 @@
         <v>45</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>335</v>
+        <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>249</v>
+        <v>329</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5603,7 +5608,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5614,7 +5619,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
@@ -5629,16 +5634,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5663,13 +5668,13 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
@@ -5687,31 +5692,31 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AF36" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>335</v>
-      </c>
       <c r="AL36" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5722,7 +5727,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5733,7 +5738,7 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5745,17 +5750,19 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>345</v>
+        <v>142</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>342</v>
+      </c>
       <c r="N37" t="s" s="2">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5780,13 +5787,13 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>45</v>
+        <v>344</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>45</v>
+        <v>345</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5804,13 +5811,13 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>45</v>
@@ -5822,13 +5829,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>45</v>
+        <v>337</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>349</v>
+        <v>251</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5839,7 +5846,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5862,16 +5869,18 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>252</v>
+        <v>347</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="N38" t="s" s="2">
+        <v>350</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5919,7 +5928,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5940,10 +5949,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>322</v>
+        <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5954,7 +5963,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5965,7 +5974,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -5974,23 +5983,19 @@
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>358</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6038,19 +6043,19 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>45</v>
@@ -6059,10 +6064,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>360</v>
+        <v>324</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6073,7 +6078,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6084,7 +6089,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6093,19 +6098,23 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>306</v>
+        <v>357</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6153,19 +6162,19 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6174,10 +6183,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>309</v>
+        <v>363</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6188,18 +6197,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6211,17 +6220,15 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6270,13 +6277,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6294,7 +6301,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6305,11 +6312,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6322,19 +6329,19 @@
         <v>45</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6387,7 +6394,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6411,7 +6418,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6422,43 +6429,41 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>366</v>
+        <v>108</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>367</v>
+        <v>317</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>369</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6482,13 +6487,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>371</v>
+        <v>45</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6506,13 +6511,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>365</v>
+        <v>318</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6527,10 +6532,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>372</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6541,7 +6546,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6549,7 +6554,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>56</v>
@@ -6564,16 +6569,20 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>374</v>
+        <v>75</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>371</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6597,13 +6606,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>45</v>
+        <v>372</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6621,10 +6630,10 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>56</v>
@@ -6642,10 +6651,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6656,7 +6665,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6664,10 +6673,10 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6676,23 +6685,19 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>297</v>
+        <v>376</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>382</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6740,19 +6745,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6761,10 +6766,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>383</v>
+        <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6775,7 +6780,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6786,7 +6791,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6795,19 +6800,23 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>306</v>
+        <v>381</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>384</v>
+      </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6855,19 +6864,19 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>308</v>
+        <v>380</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6876,10 +6885,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>45</v>
+        <v>385</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>309</v>
+        <v>386</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6890,18 +6899,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
@@ -6913,17 +6922,15 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6972,13 +6979,13 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
@@ -6996,7 +7003,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7007,11 +7014,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7024,19 +7031,19 @@
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7089,7 +7096,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7113,7 +7120,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>99</v>
+        <v>311</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7124,41 +7131,41 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>57</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>389</v>
+        <v>108</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" t="s" s="2">
-        <v>156</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7182,13 +7189,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7206,13 +7213,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>388</v>
+        <v>318</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7224,16 +7231,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>391</v>
+        <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>163</v>
+        <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>164</v>
+        <v>99</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7241,7 +7248,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7249,7 +7256,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>56</v>
@@ -7264,19 +7271,17 @@
         <v>57</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>393</v>
+        <v>142</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>395</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7301,13 +7306,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7325,10 +7330,10 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>56</v>
@@ -7343,24 +7348,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>228</v>
+        <v>163</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>229</v>
+        <v>164</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>230</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7380,22 +7385,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>142</v>
+        <v>395</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7420,13 +7425,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>236</v>
+        <v>45</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7444,7 +7449,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7453,7 +7458,7 @@
         <v>56</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>238</v>
+        <v>45</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>45</v>
@@ -7462,28 +7467,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>45</v>
+        <v>398</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>99</v>
+        <v>227</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>45</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7505,16 +7510,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>242</v>
+        <v>400</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7542,10 +7547,10 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7563,7 +7568,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7572,7 +7577,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7581,19 +7586,19 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>248</v>
+        <v>99</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" hidden="true">
@@ -7602,14 +7607,14 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7621,19 +7626,19 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L53" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>300</v>
-      </c>
       <c r="N53" t="s" s="2">
-        <v>301</v>
+        <v>246</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7658,13 +7663,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7688,35 +7693,154 @@
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F54" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="AH53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL53" t="s" s="2">
+      <c r="G54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="N54" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="AM53" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO53" t="s" s="2">
+      <c r="O54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO54" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO53">
+  <autoFilter ref="A1:AO54">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7726,7 +7850,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI52">
+  <conditionalFormatting sqref="A2:AI53">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated outputs for below implementation guides which has an update to their corresponding ig.xml files.
- Advance Care Records
- Event Summary
- Personal Health Records
- Prescription and Dispense Lists
- Shared health Summary

CIFMM-2490
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="404">
   <si>
     <t>Path</t>
   </si>
@@ -702,10 +702,13 @@
     <t>who.actor</t>
   </si>
   <si>
-    <t>Observation.value[x]</t>
-  </si>
-  <si>
-    <t>Actual result</t>
+    <t>Observation.valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Coded value of the observation</t>
   </si>
   <si>
     <t>The information determined as a result of making the observation, if the information has a simple value.</t>
@@ -720,11 +723,10 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
+  </si>
+  <si>
+    <t>Observation.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -744,15 +746,6 @@
   </si>
   <si>
     <t>363714003 |Interprets|</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Coded value of the observation</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1441,7 +1434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO54"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3849,23 +3842,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" t="s" s="2">
+        <v>218</v>
+      </c>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3877,16 +3872,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3911,29 +3906,29 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X21" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="X21" s="2"/>
       <c r="Y21" t="s" s="2">
-        <v>45</v>
+        <v>223</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AB21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>223</v>
+        <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3942,70 +3937,68 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4030,11 +4023,13 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X22" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="Y22" t="s" s="2">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4052,7 +4047,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4061,44 +4056,44 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>227</v>
+        <v>99</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>229</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4113,16 +4108,14 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4150,10 +4143,10 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4171,7 +4164,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4180,37 +4173,37 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>99</v>
+        <v>248</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>243</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4229,17 +4222,17 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4264,13 +4257,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4288,7 +4281,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4303,27 +4296,27 @@
         <v>45</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>252</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4346,18 +4339,18 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>254</v>
+        <v>142</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" t="s" s="2">
-        <v>257</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4381,13 +4374,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4405,7 +4398,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4420,27 +4413,27 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>45</v>
+        <v>265</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4466,15 +4459,17 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N26" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4501,10 +4496,10 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4522,7 +4517,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4540,24 +4535,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4580,20 +4575,18 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>275</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4617,13 +4610,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>277</v>
+        <v>45</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4641,7 +4634,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4659,24 +4652,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>45</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4699,16 +4692,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4758,7 +4751,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4776,24 +4769,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4804,7 +4797,7 @@
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4816,18 +4809,20 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4875,42 +4870,42 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>297</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4921,7 +4916,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -4933,20 +4928,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>303</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -4994,19 +4985,19 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>304</v>
+        <v>45</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>45</v>
@@ -5015,10 +5006,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>305</v>
+        <v>45</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5029,18 +5020,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5052,15 +5043,17 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5109,13 +5102,13 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
@@ -5133,7 +5126,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5144,11 +5137,11 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -5161,19 +5154,19 @@
         <v>45</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J32" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5226,7 +5219,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5250,7 +5243,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5261,40 +5254,38 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>102</v>
+        <v>318</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>108</v>
+        <v>319</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5343,16 +5334,16 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>45</v>
@@ -5364,10 +5355,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>45</v>
+        <v>322</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>99</v>
+        <v>323</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5378,7 +5369,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5401,13 +5392,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5458,7 +5449,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5467,7 +5458,7 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>45</v>
@@ -5479,10 +5470,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5493,7 +5484,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5516,16 +5507,20 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>320</v>
+        <v>142</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>332</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5549,13 +5544,13 @@
         <v>45</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>45</v>
+        <v>334</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>45</v>
@@ -5573,7 +5568,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5582,7 +5577,7 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>323</v>
+        <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>45</v>
@@ -5591,13 +5586,13 @@
         <v>45</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>45</v>
+        <v>335</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>329</v>
+        <v>249</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5608,7 +5603,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5619,7 +5614,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
@@ -5634,16 +5629,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5668,55 +5663,55 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE36" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="Y36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="Z36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="AF36" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="AL36" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="AM36" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5727,7 +5722,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5738,7 +5733,7 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5750,19 +5745,17 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>142</v>
+        <v>345</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>342</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5787,37 +5780,37 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE37" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>339</v>
-      </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>45</v>
@@ -5829,13 +5822,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>337</v>
+        <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>338</v>
+        <v>45</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>251</v>
+        <v>349</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5846,7 +5839,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5869,18 +5862,16 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>347</v>
+        <v>252</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="M38" s="2"/>
-      <c r="N38" t="s" s="2">
-        <v>350</v>
-      </c>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5928,7 +5919,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5949,10 +5940,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>45</v>
+        <v>322</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5963,7 +5954,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5974,7 +5965,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -5983,19 +5974,23 @@
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>358</v>
+      </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6043,19 +6038,19 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>45</v>
@@ -6064,10 +6059,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6078,7 +6073,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6089,7 +6084,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6098,23 +6093,19 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>357</v>
+        <v>306</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6162,19 +6153,19 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6183,10 +6174,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>362</v>
+        <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>363</v>
+        <v>309</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6197,18 +6188,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6220,15 +6211,17 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6277,13 +6270,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6301,7 +6294,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6312,11 +6305,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6329,19 +6322,19 @@
         <v>45</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J42" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6394,7 +6387,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6418,7 +6411,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6429,41 +6422,43 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>108</v>
+        <v>366</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>367</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N43" s="2"/>
+        <v>368</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>369</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6487,13 +6482,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>45</v>
+        <v>370</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>45</v>
+        <v>371</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6511,13 +6506,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>318</v>
+        <v>365</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6532,10 +6527,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>99</v>
+        <v>372</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6546,7 +6541,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6554,7 +6549,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>56</v>
@@ -6569,20 +6564,16 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>75</v>
+        <v>374</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>371</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6606,34 +6597,34 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>372</v>
+        <v>45</v>
       </c>
       <c r="Y44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE44" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="Z44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>367</v>
-      </c>
       <c r="AF44" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>56</v>
@@ -6651,10 +6642,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6665,7 +6656,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6673,10 +6664,10 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6685,19 +6676,23 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>376</v>
+        <v>297</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>380</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>382</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6745,19 +6740,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6766,10 +6761,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>45</v>
+        <v>383</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6780,7 +6775,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6791,7 +6786,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6800,23 +6795,19 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>381</v>
+        <v>306</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>384</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6864,19 +6855,19 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>380</v>
+        <v>308</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6885,10 +6876,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>385</v>
+        <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>386</v>
+        <v>309</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6899,18 +6890,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
@@ -6922,15 +6913,17 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>254</v>
+        <v>102</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>308</v>
+        <v>103</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M47" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6979,13 +6972,13 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
@@ -7003,7 +6996,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7014,11 +7007,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>101</v>
+        <v>314</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7031,19 +7024,19 @@
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="J48" t="s" s="2">
         <v>102</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7096,7 +7089,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7120,7 +7113,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7131,41 +7124,41 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>57</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>108</v>
+        <v>389</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N49" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7189,13 +7182,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7213,13 +7206,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7231,16 +7224,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>45</v>
+        <v>391</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7248,7 +7241,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7256,7 +7249,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>56</v>
@@ -7271,17 +7264,19 @@
         <v>57</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>142</v>
+        <v>393</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="M50" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>395</v>
+      </c>
       <c r="N50" t="s" s="2">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7306,13 +7301,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7330,10 +7325,10 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>56</v>
@@ -7348,24 +7343,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7385,22 +7380,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>395</v>
+        <v>142</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7425,13 +7420,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>45</v>
+        <v>236</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>45</v>
+        <v>237</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7449,7 +7444,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7458,7 +7453,7 @@
         <v>56</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>45</v>
@@ -7467,28 +7462,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>398</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>227</v>
+        <v>99</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>229</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7510,16 +7505,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>400</v>
+        <v>242</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7547,10 +7542,10 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7568,7 +7563,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7577,7 +7572,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7586,19 +7581,19 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>99</v>
+        <v>248</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" hidden="true">
@@ -7607,14 +7602,14 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>243</v>
+        <v>45</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7626,19 +7621,19 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>244</v>
+        <v>403</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>403</v>
+        <v>300</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>246</v>
+        <v>301</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7663,13 +7658,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7693,7 +7688,7 @@
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>45</v>
@@ -7705,142 +7700,23 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>251</v>
+        <v>304</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO54" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO54">
+  <autoFilter ref="A1:AO53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7850,7 +7726,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI53">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated  invariants STU3 Observation  Assertion of No Relevant Finding - CIFMM-2699. Regenerated ouptuts for ES, PHR, SHS and SML.
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="405">
   <si>
     <t>Path</t>
   </si>
@@ -166,7 +166,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or code!=component.code}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or code!=component.code}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}inv-dh-obs-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-obs-02:If present, a performer shall at least have a reference, an identifier or a display {performer.exists() implies performer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
   </si>
   <si>
     <t>Event</t>
@@ -561,10 +561,6 @@
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-obs-01:The subject shall at least have a reference or an identifier {reference.exists() or identifier.exists()}
-</t>
   </si>
   <si>
     <t>Event.subject</t>
@@ -3356,22 +3352,22 @@
         <v>45</v>
       </c>
       <c r="AI16" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AJ16" t="s" s="2">
+      <c r="AK16" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL16" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AK16" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3379,11 +3375,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3402,19 +3398,19 @@
         <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>183</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>184</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3463,7 +3459,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3478,19 +3474,19 @@
         <v>45</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3498,11 +3494,11 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3521,19 +3517,19 @@
         <v>57</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>193</v>
       </c>
-      <c r="M18" t="s" s="2">
+      <c r="N18" t="s" s="2">
         <v>194</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>195</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3582,7 +3578,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3597,19 +3593,19 @@
         <v>45</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="AK18" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="AM18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>198</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>199</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3617,7 +3613,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3640,16 +3636,16 @@
         <v>57</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3699,7 +3695,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3720,13 +3716,13 @@
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="AM19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3734,7 +3730,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3757,17 +3753,17 @@
         <v>57</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>211</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3816,7 +3812,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3831,19 +3827,19 @@
         <v>45</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="AK20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL20" t="s" s="2">
+      <c r="AM20" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AN20" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3851,7 +3847,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3877,16 +3873,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3923,17 +3919,17 @@
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3942,36 +3938,36 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="AI21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AK21" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>45</v>
@@ -3996,16 +3992,16 @@
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L22" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4034,7 +4030,7 @@
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4052,7 +4048,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4061,33 +4057,33 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="AI22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AK22" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO22" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4113,16 +4109,16 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>236</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4150,11 +4146,11 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="Y23" t="s" s="2">
-        <v>239</v>
-      </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
       </c>
@@ -4171,7 +4167,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4180,13 +4176,13 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
@@ -4195,7 +4191,7 @@
         <v>99</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
@@ -4206,11 +4202,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4232,14 +4228,14 @@
         <v>142</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4267,11 +4263,11 @@
         <v>79</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="Y24" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>248</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4288,7 +4284,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4306,24 +4302,24 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AL24" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AL24" t="s" s="2">
+      <c r="AM24" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="AM24" t="s" s="2">
+      <c r="AN24" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO24" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO24" t="s" s="2">
-        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4346,17 +4342,17 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4405,7 +4401,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4420,16 +4416,16 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AK25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="AM25" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
@@ -4440,7 +4436,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4466,13 +4462,13 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>264</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -4501,11 +4497,11 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="Y26" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="Y26" t="s" s="2">
-        <v>266</v>
-      </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4522,7 +4518,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4540,24 +4536,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AL26" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="AL26" t="s" s="2">
+      <c r="AM26" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="AM26" t="s" s="2">
+      <c r="AN26" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO26" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO26" t="s" s="2">
-        <v>270</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4583,16 +4579,16 @@
         <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4620,11 +4616,11 @@
         <v>158</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="Y27" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>277</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4641,7 +4637,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4662,10 +4658,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>278</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>279</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -4676,7 +4672,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4699,16 +4695,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="K28" t="s" s="2">
+      <c r="L28" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4758,7 +4754,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4776,24 +4772,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AL28" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AL28" t="s" s="2">
+      <c r="AM28" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AM28" t="s" s="2">
+      <c r="AN28" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO28" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AN28" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO28" t="s" s="2">
-        <v>288</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4816,16 +4812,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4875,7 +4871,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4893,24 +4889,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>297</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4933,19 +4929,19 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -4994,7 +4990,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5006,19 +5002,19 @@
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="AJ30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5029,7 +5025,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5052,13 +5048,13 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5109,7 +5105,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5133,7 +5129,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5144,7 +5140,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5173,7 +5169,7 @@
         <v>103</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5226,7 +5222,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5250,7 +5246,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5261,11 +5257,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -5290,7 +5286,7 @@
         <v>108</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>105</v>
@@ -5343,7 +5339,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5378,7 +5374,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5401,13 +5397,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5458,7 +5454,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5467,22 +5463,22 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL34" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="AI34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL34" t="s" s="2">
+      <c r="AM34" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5493,7 +5489,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5516,13 +5512,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5573,7 +5569,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5582,22 +5578,22 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="AI35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>324</v>
-      </c>
       <c r="AM35" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5608,7 +5604,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5634,16 +5630,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5671,11 +5667,11 @@
         <v>79</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="Y36" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>336</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5692,7 +5688,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5710,13 +5706,13 @@
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AL36" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="AM36" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5727,7 +5723,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5753,16 +5749,16 @@
         <v>142</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5790,11 +5786,11 @@
         <v>158</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>345</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5811,7 +5807,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5829,13 +5825,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="AL37" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="AM37" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5846,7 +5842,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5869,17 +5865,17 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="K38" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="K38" t="s" s="2">
+      <c r="L38" t="s" s="2">
         <v>348</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>349</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5928,7 +5924,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5952,7 +5948,7 @@
         <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5963,7 +5959,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5986,13 +5982,13 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6043,7 +6039,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6064,10 +6060,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6078,7 +6074,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6101,19 +6097,19 @@
         <v>57</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>360</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6162,7 +6158,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6174,19 +6170,19 @@
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>361</v>
       </c>
-      <c r="AJ40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL40" t="s" s="2">
+      <c r="AM40" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6197,7 +6193,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6220,13 +6216,13 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6277,7 +6273,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6301,7 +6297,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6312,7 +6308,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6341,7 +6337,7 @@
         <v>103</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6394,7 +6390,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6418,7 +6414,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6429,11 +6425,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6458,7 +6454,7 @@
         <v>108</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M43" t="s" s="2">
         <v>105</v>
@@ -6511,7 +6507,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6546,7 +6542,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6572,16 +6568,16 @@
         <v>75</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6609,11 +6605,11 @@
         <v>133</v>
       </c>
       <c r="X44" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="Y44" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="Y44" t="s" s="2">
-        <v>373</v>
-      </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6630,7 +6626,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6654,7 +6650,7 @@
         <v>99</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6665,7 +6661,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6688,13 +6684,13 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="L45" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6745,7 +6741,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>56</v>
@@ -6769,7 +6765,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6780,7 +6776,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6803,19 +6799,19 @@
         <v>57</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="M46" t="s" s="2">
+      <c r="N46" t="s" s="2">
         <v>383</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -6864,7 +6860,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6876,7 +6872,7 @@
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6885,10 +6881,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6899,7 +6895,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6922,13 +6918,13 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6979,7 +6975,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7003,7 +6999,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7014,7 +7010,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7043,7 +7039,7 @@
         <v>103</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7096,7 +7092,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7120,7 +7116,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7131,11 +7127,11 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7160,7 +7156,7 @@
         <v>108</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>105</v>
@@ -7213,7 +7209,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7248,7 +7244,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7274,10 +7270,10 @@
         <v>142</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
@@ -7330,7 +7326,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>56</v>
@@ -7348,7 +7344,7 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>163</v>
@@ -7365,7 +7361,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7388,19 +7384,19 @@
         <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="L51" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>397</v>
-      </c>
       <c r="N51" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7449,7 +7445,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7467,24 +7463,24 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AM51" t="s" s="2">
+      <c r="AN51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO51" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7510,16 +7506,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="L52" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>401</v>
-      </c>
       <c r="N52" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7547,11 +7543,11 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="Y52" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="Y52" t="s" s="2">
-        <v>239</v>
-      </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
       </c>
@@ -7568,7 +7564,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7577,7 +7573,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7592,7 +7588,7 @@
         <v>99</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7603,11 +7599,11 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7629,16 +7625,16 @@
         <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="N53" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7666,11 +7662,11 @@
         <v>79</v>
       </c>
       <c r="X53" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="Y53" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Y53" t="s" s="2">
-        <v>248</v>
-      </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
       </c>
@@ -7687,7 +7683,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7705,24 +7701,24 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AL53" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AL53" t="s" s="2">
+      <c r="AM53" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="AM53" t="s" s="2">
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO53" t="s" s="2">
-        <v>252</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7748,16 +7744,16 @@
         <v>45</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L54" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -7806,7 +7802,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -7827,10 +7823,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Build IGs folllowing completion of task and commit output
</commit_message>
<xml_diff>
--- a/output/EventSummary/observation-norelevantfinding-1.xlsx
+++ b/output/EventSummary/observation-norelevantfinding-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="406">
   <si>
     <t>Path</t>
   </si>
@@ -166,7 +166,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or code!=component.code}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}inv-dh-obs-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-obs-02:If present, a performer shall at least have a reference, an identifier or a display {performer.exists() implies performer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or code!=component.code}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -561,6 +561,10 @@
   </si>
   <si>
     <t>Observations have no value if you don't know who or what they're about.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv-dh-obs-01:The subject shall at least have a reference or an identifier {reference.exists() or identifier.exists()}
+</t>
   </si>
   <si>
     <t>Event.subject</t>
@@ -3352,22 +3356,22 @@
         <v>45</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3375,11 +3379,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3398,19 +3402,19 @@
         <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3459,7 +3463,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3474,19 +3478,19 @@
         <v>45</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3494,11 +3498,11 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3517,19 +3521,19 @@
         <v>57</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3578,7 +3582,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3593,19 +3597,19 @@
         <v>45</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3613,7 +3617,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3636,16 +3640,16 @@
         <v>57</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3695,7 +3699,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3716,13 +3720,13 @@
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3730,7 +3734,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3753,17 +3757,17 @@
         <v>57</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3812,7 +3816,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3827,19 +3831,19 @@
         <v>45</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3847,7 +3851,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3873,16 +3877,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3919,17 +3923,17 @@
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3938,36 +3942,36 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>45</v>
@@ -3992,16 +3996,16 @@
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4030,7 +4034,7 @@
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4048,7 +4052,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4057,33 +4061,33 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4109,16 +4113,16 @@
         <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4146,10 +4150,10 @@
         <v>79</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4167,7 +4171,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4176,13 +4180,13 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
@@ -4191,7 +4195,7 @@
         <v>99</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
@@ -4202,11 +4206,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4228,14 +4232,14 @@
         <v>142</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4263,10 +4267,10 @@
         <v>79</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4284,7 +4288,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4302,24 +4306,24 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4342,17 +4346,17 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4401,7 +4405,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4416,16 +4420,16 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
@@ -4436,7 +4440,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4462,13 +4466,13 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -4497,10 +4501,10 @@
         <v>158</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4518,7 +4522,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4536,24 +4540,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4579,16 +4583,16 @@
         <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4616,10 +4620,10 @@
         <v>158</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4637,7 +4641,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4658,10 +4662,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -4672,7 +4676,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4695,16 +4699,16 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4754,7 +4758,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4772,24 +4776,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4812,16 +4816,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4871,7 +4875,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4889,24 +4893,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4929,19 +4933,19 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -4990,7 +4994,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5002,7 +5006,7 @@
         <v>45</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>45</v>
@@ -5011,10 +5015,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5025,7 +5029,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5048,13 +5052,13 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5105,7 +5109,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5129,7 +5133,7 @@
         <v>45</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5140,7 +5144,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5169,7 +5173,7 @@
         <v>103</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>105</v>
@@ -5222,7 +5226,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5246,7 +5250,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5257,11 +5261,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -5286,7 +5290,7 @@
         <v>108</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>105</v>
@@ -5339,7 +5343,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5374,7 +5378,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5397,13 +5401,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5454,7 +5458,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5463,7 +5467,7 @@
         <v>56</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>45</v>
@@ -5475,10 +5479,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5489,7 +5493,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5512,13 +5516,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5569,7 +5573,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5578,7 +5582,7 @@
         <v>56</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>45</v>
@@ -5590,10 +5594,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5604,7 +5608,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5630,16 +5634,16 @@
         <v>142</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5667,10 +5671,10 @@
         <v>79</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
@@ -5688,7 +5692,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5706,13 +5710,13 @@
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5723,7 +5727,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5749,16 +5753,16 @@
         <v>142</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5786,10 +5790,10 @@
         <v>158</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5807,7 +5811,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5825,13 +5829,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5842,7 +5846,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5865,17 +5869,17 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5924,7 +5928,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5948,7 +5952,7 @@
         <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5959,7 +5963,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5982,13 +5986,13 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6039,7 +6043,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6060,10 +6064,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6074,7 +6078,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6097,19 +6101,19 @@
         <v>57</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6158,7 +6162,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6170,7 +6174,7 @@
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6179,10 +6183,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6193,7 +6197,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6216,13 +6220,13 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6273,7 +6277,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6297,7 +6301,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6308,7 +6312,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6337,7 +6341,7 @@
         <v>103</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>105</v>
@@ -6390,7 +6394,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6414,7 +6418,7 @@
         <v>45</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6425,11 +6429,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6454,7 +6458,7 @@
         <v>108</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M43" t="s" s="2">
         <v>105</v>
@@ -6507,7 +6511,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6542,7 +6546,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6568,16 +6572,16 @@
         <v>75</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6605,10 +6609,10 @@
         <v>133</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6626,7 +6630,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6650,7 +6654,7 @@
         <v>99</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6661,7 +6665,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6684,13 +6688,13 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6741,7 +6745,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>56</v>
@@ -6765,7 +6769,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6776,7 +6780,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6799,19 +6803,19 @@
         <v>57</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -6860,7 +6864,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6872,7 +6876,7 @@
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6881,10 +6885,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6895,7 +6899,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6918,13 +6922,13 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6975,7 +6979,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -6999,7 +7003,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7010,7 +7014,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7039,7 +7043,7 @@
         <v>103</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>105</v>
@@ -7092,7 +7096,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7116,7 +7120,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7127,11 +7131,11 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7156,7 +7160,7 @@
         <v>108</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>105</v>
@@ -7209,7 +7213,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7244,7 +7248,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7270,10 +7274,10 @@
         <v>142</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
@@ -7326,7 +7330,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>56</v>
@@ -7344,7 +7348,7 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>163</v>
@@ -7361,7 +7365,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7384,19 +7388,19 @@
         <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7445,7 +7449,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7463,24 +7467,24 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7506,16 +7510,16 @@
         <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7543,10 +7547,10 @@
         <v>79</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7564,7 +7568,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7573,7 +7577,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7588,7 +7592,7 @@
         <v>99</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7599,11 +7603,11 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7625,16 +7629,16 @@
         <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7662,10 +7666,10 @@
         <v>79</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7683,7 +7687,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7701,24 +7705,24 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7744,16 +7748,16 @@
         <v>45</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -7802,7 +7806,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -7823,10 +7827,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>

</xml_diff>